<commit_message>
all MGTs except two quads used for c2c
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
+++ b/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="US+_GTY_tx_rx" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7034" uniqueCount="1607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="1607">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -2573,13 +2573,13 @@
     <t xml:space="preserve">s</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">out</t>
   </si>
   <si>
     <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
@@ -11618,8 +11618,8 @@
   </sheetPr>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11787,6 +11787,9 @@
       <c r="E8" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="J8" s="4" t="s">
+        <v>848</v>
+      </c>
       <c r="L8" s="0"/>
       <c r="M8" s="5"/>
     </row>
@@ -11795,7 +11798,7 @@
         <v>739</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>847</v>
@@ -11804,10 +11807,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="5"/>
@@ -11817,7 +11820,7 @@
         <v>740</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>847</v>
@@ -11826,10 +11829,10 @@
         <v>1</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="5"/>
@@ -11848,7 +11851,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="5"/>
@@ -11870,7 +11873,7 @@
         <v>852</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="5"/>
@@ -11889,10 +11892,10 @@
         <v>1</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="5"/>
@@ -11902,7 +11905,7 @@
         <v>741</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>847</v>
@@ -11911,10 +11914,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="5"/>
@@ -11936,7 +11939,7 @@
         <v>853</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="5"/>
@@ -11997,7 +12000,7 @@
         <v>742</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>0</v>
@@ -12006,7 +12009,7 @@
         <v>16</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="5"/>
@@ -12016,7 +12019,7 @@
         <v>743</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>0</v>
@@ -12025,7 +12028,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L20" s="0"/>
       <c r="M20" s="5"/>
@@ -12095,7 +12098,7 @@
         <v>744</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>854</v>
@@ -12110,7 +12113,7 @@
         <v>855</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L24" s="0"/>
       <c r="M24" s="5"/>
@@ -12142,7 +12145,7 @@
         <v>745</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>854</v>
@@ -12157,7 +12160,7 @@
         <v>855</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L26" s="0"/>
       <c r="M26" s="5"/>
@@ -12205,7 +12208,7 @@
         <v>746</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>847</v>
@@ -12214,7 +12217,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="5"/>
@@ -12233,7 +12236,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L30" s="0"/>
       <c r="M30" s="5"/>
@@ -12287,7 +12290,7 @@
         <v>1</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L33" s="0"/>
       <c r="M33" s="5"/>
@@ -12306,7 +12309,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L34" s="0"/>
       <c r="M34" s="5"/>
@@ -12325,7 +12328,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L35" s="0"/>
       <c r="M35" s="5"/>
@@ -12335,7 +12338,7 @@
         <v>747</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>847</v>
@@ -12344,7 +12347,10 @@
         <v>1</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>848</v>
       </c>
       <c r="L36" s="0"/>
       <c r="M36" s="5"/>
@@ -12363,7 +12369,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L37" s="0"/>
       <c r="M37" s="5"/>
@@ -12382,7 +12388,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L38" s="0"/>
       <c r="M38" s="5"/>
@@ -12392,16 +12398,16 @@
         <v>748</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>848</v>
-      </c>
-      <c r="C39" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>850</v>
       </c>
       <c r="L39" s="0"/>
       <c r="M39" s="5"/>
@@ -12420,7 +12426,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L40" s="0"/>
       <c r="M40" s="5"/>
@@ -12439,7 +12445,10 @@
         <v>1</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>848</v>
       </c>
       <c r="L41" s="0"/>
       <c r="M41" s="5"/>
@@ -12458,7 +12467,7 @@
         <v>1</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L42" s="0"/>
       <c r="M42" s="5"/>
@@ -12477,7 +12486,7 @@
         <v>1</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L43" s="0"/>
       <c r="M43" s="5"/>
@@ -12496,7 +12505,10 @@
         <v>1</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>848</v>
       </c>
       <c r="L44" s="0"/>
       <c r="M44" s="5"/>
@@ -12515,7 +12527,10 @@
         <v>1</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>848</v>
       </c>
       <c r="L45" s="0"/>
       <c r="M45" s="5"/>
@@ -12591,7 +12606,7 @@
         <v>3</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L49" s="0"/>
       <c r="M49" s="5"/>
@@ -12601,7 +12616,7 @@
         <v>749</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>856</v>
@@ -12620,7 +12635,7 @@
         <v>750</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>856</v>
@@ -12639,7 +12654,7 @@
         <v>759</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>0</v>
@@ -12655,7 +12670,7 @@
         <v>760</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>0</v>
@@ -12680,10 +12695,10 @@
         <v>1</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L54" s="0"/>
       <c r="M54" s="5"/>
@@ -12702,10 +12717,10 @@
         <v>1</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L55" s="0"/>
       <c r="M55" s="5"/>
@@ -12724,10 +12739,10 @@
         <v>1</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L56" s="0"/>
       <c r="M56" s="5"/>
@@ -12746,10 +12761,10 @@
         <v>1</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L57" s="0"/>
       <c r="M57" s="5"/>
@@ -12759,7 +12774,7 @@
         <v>763</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>0</v>
@@ -12783,6 +12798,9 @@
       <c r="E59" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="J59" s="4" t="s">
+        <v>848</v>
+      </c>
       <c r="L59" s="0"/>
       <c r="M59" s="5"/>
     </row>
@@ -12845,7 +12863,7 @@
         <v>764</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>847</v>
@@ -12857,7 +12875,7 @@
         <v>3</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L63" s="0"/>
       <c r="M63" s="5"/>
@@ -12867,7 +12885,7 @@
         <v>765</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>847</v>
@@ -12879,7 +12897,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L64" s="0"/>
       <c r="M64" s="5"/>
@@ -12889,7 +12907,7 @@
         <v>766</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>0</v>
@@ -12901,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L65" s="0"/>
       <c r="M65" s="5"/>
@@ -12943,7 +12961,7 @@
         <v>767</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>0</v>
@@ -12978,7 +12996,7 @@
         <v>768</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>0</v>
@@ -13013,7 +13031,7 @@
         <v>769</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C72" s="4" t="n">
         <v>0</v>
@@ -13032,7 +13050,7 @@
         <v>770</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C73" s="4" t="n">
         <v>0</v>
@@ -13051,7 +13069,7 @@
         <v>771</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C74" s="4" t="n">
         <v>0</v>
@@ -13146,7 +13164,7 @@
         <v>772</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>0</v>
@@ -13184,7 +13202,7 @@
         <v>773</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C81" s="4" t="n">
         <v>0</v>
@@ -13232,7 +13250,7 @@
         <v>774</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C84" s="4" t="n">
         <v>0</v>
@@ -13251,7 +13269,7 @@
         <v>775</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C85" s="4" t="n">
         <v>0</v>
@@ -13270,7 +13288,7 @@
         <v>776</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C86" s="4" t="n">
         <v>0</v>
@@ -13282,7 +13300,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L86" s="0"/>
       <c r="M86" s="5"/>
@@ -13311,7 +13329,7 @@
         <v>777</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C88" s="4" t="n">
         <v>0</v>
@@ -13330,7 +13348,7 @@
         <v>778</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C89" s="4" t="n">
         <v>0</v>
@@ -13349,7 +13367,7 @@
         <v>779</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>856</v>
@@ -13364,7 +13382,7 @@
         <v>857</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L90" s="0"/>
       <c r="M90" s="5"/>
@@ -13374,7 +13392,7 @@
         <v>780</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>856</v>
@@ -13389,7 +13407,7 @@
         <v>857</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L91" s="0"/>
       <c r="M91" s="5"/>
@@ -13399,7 +13417,7 @@
         <v>781</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>856</v>
@@ -13414,7 +13432,7 @@
         <v>857</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L92" s="0"/>
       <c r="M92" s="5"/>
@@ -13424,7 +13442,7 @@
         <v>782</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>856</v>
@@ -13439,7 +13457,7 @@
         <v>857</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L93" s="0"/>
       <c r="M93" s="5"/>
@@ -13449,7 +13467,7 @@
         <v>783</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>856</v>
@@ -13464,7 +13482,7 @@
         <v>857</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L94" s="0"/>
       <c r="M94" s="5"/>
@@ -13474,7 +13492,7 @@
         <v>784</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C95" s="4" t="n">
         <v>0</v>
@@ -13493,7 +13511,7 @@
         <v>785</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>856</v>
@@ -13508,7 +13526,7 @@
         <v>857</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L96" s="0"/>
       <c r="M96" s="5"/>
@@ -13736,7 +13754,7 @@
         <v>1</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L108" s="0"/>
       <c r="M108" s="2"/>
@@ -14437,7 +14455,7 @@
         <v>786</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>847</v>
@@ -14446,7 +14464,7 @@
         <v>1</v>
       </c>
       <c r="H146" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L146" s="0"/>
       <c r="M146" s="5"/>
@@ -14456,7 +14474,7 @@
         <v>787</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C147" s="4" t="n">
         <v>0</v>
@@ -14503,7 +14521,7 @@
         <v>857</v>
       </c>
       <c r="H149" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L149" s="0"/>
       <c r="M149" s="5"/>
@@ -14513,7 +14531,7 @@
         <v>788</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>856</v>
@@ -14528,7 +14546,7 @@
         <v>857</v>
       </c>
       <c r="H150" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L150" s="0"/>
       <c r="M150" s="5"/>
@@ -14538,7 +14556,7 @@
         <v>789</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>856</v>
@@ -14553,7 +14571,7 @@
         <v>857</v>
       </c>
       <c r="H151" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L151" s="0"/>
       <c r="M151" s="5"/>
@@ -14769,7 +14787,7 @@
         <v>793</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C163" s="4" t="n">
         <v>0</v>
@@ -14829,7 +14847,7 @@
         <v>1</v>
       </c>
       <c r="H166" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L166" s="5"/>
       <c r="M166" s="5"/>
@@ -14858,7 +14876,7 @@
         <v>794</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C168" s="4" t="n">
         <v>0</v>
@@ -14874,7 +14892,7 @@
         <v>795</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C169" s="4" t="n">
         <v>0</v>
@@ -14890,7 +14908,7 @@
         <v>796</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C170" s="4" t="n">
         <v>0</v>
@@ -14906,7 +14924,7 @@
         <v>797</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C171" s="4" t="n">
         <v>0</v>
@@ -14941,7 +14959,7 @@
         <v>798</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>851</v>
@@ -14953,7 +14971,7 @@
         <v>857</v>
       </c>
       <c r="H173" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="I173" s="4" t="s">
         <v>861</v>
@@ -14966,7 +14984,7 @@
         <v>799</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C174" s="4" t="n">
         <v>0</v>
@@ -14975,7 +14993,7 @@
         <v>1</v>
       </c>
       <c r="H174" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L174" s="5"/>
       <c r="M174" s="8"/>
@@ -14985,7 +15003,7 @@
         <v>800</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C175" s="4" t="n">
         <v>0</v>
@@ -14994,7 +15012,7 @@
         <v>1</v>
       </c>
       <c r="H175" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L175" s="5"/>
       <c r="M175" s="0"/>
@@ -15048,7 +15066,7 @@
         <v>1</v>
       </c>
       <c r="H178" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L178" s="2"/>
       <c r="M178" s="0"/>
@@ -15070,7 +15088,7 @@
         <v>862</v>
       </c>
       <c r="H179" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L179" s="5"/>
       <c r="M179" s="0"/>
@@ -15096,7 +15114,7 @@
         <v>801</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>856</v>
@@ -15105,7 +15123,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L181" s="5"/>
       <c r="M181" s="0"/>
@@ -15131,7 +15149,7 @@
         <v>802</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>847</v>
@@ -15140,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="H183" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L183" s="5"/>
       <c r="M183" s="0"/>
@@ -15191,10 +15209,10 @@
         <v>2</v>
       </c>
       <c r="H186" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J186" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L186" s="5"/>
       <c r="M186" s="0"/>
@@ -15213,7 +15231,7 @@
         <v>1</v>
       </c>
       <c r="H187" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L187" s="5"/>
       <c r="M187" s="0"/>
@@ -15223,7 +15241,7 @@
         <v>803</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>847</v>
@@ -15232,7 +15250,7 @@
         <v>1</v>
       </c>
       <c r="H188" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L188" s="5"/>
       <c r="M188" s="0"/>
@@ -15277,7 +15295,7 @@
         <v>804</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>847</v>
@@ -15289,7 +15307,7 @@
         <v>1</v>
       </c>
       <c r="H191" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L191" s="5"/>
       <c r="M191" s="0"/>
@@ -15299,7 +15317,7 @@
         <v>805</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>847</v>
@@ -15311,7 +15329,7 @@
         <v>1</v>
       </c>
       <c r="H192" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L192" s="5"/>
       <c r="M192" s="0"/>
@@ -15340,7 +15358,7 @@
         <v>806</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>847</v>
@@ -15349,7 +15367,7 @@
         <v>1</v>
       </c>
       <c r="H194" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L194" s="5"/>
       <c r="M194" s="0"/>
@@ -15391,7 +15409,7 @@
         <v>807</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C197" s="4" t="n">
         <v>0</v>
@@ -15403,7 +15421,7 @@
         <v>1</v>
       </c>
       <c r="H197" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L197" s="5"/>
       <c r="M197" s="0"/>
@@ -15429,7 +15447,7 @@
         <v>809</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>847</v>
@@ -15438,7 +15456,7 @@
         <v>1</v>
       </c>
       <c r="H199" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L199" s="5"/>
       <c r="M199" s="0"/>
@@ -15502,7 +15520,7 @@
         <v>814</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>856</v>
@@ -15517,7 +15535,7 @@
         <v>857</v>
       </c>
       <c r="H203" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L203" s="5"/>
       <c r="M203" s="0"/>
@@ -15527,7 +15545,7 @@
         <v>815</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C204" s="4" t="n">
         <v>0</v>
@@ -15555,7 +15573,7 @@
         <v>816</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>847</v>
@@ -15564,7 +15582,7 @@
         <v>1</v>
       </c>
       <c r="H206" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15600,7 +15618,7 @@
         <v>817</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>847</v>
@@ -15609,7 +15627,7 @@
         <v>1</v>
       </c>
       <c r="H209" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15626,10 +15644,10 @@
         <v>2</v>
       </c>
       <c r="H210" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J210" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15663,7 +15681,7 @@
         <v>1</v>
       </c>
       <c r="H212" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15680,7 +15698,7 @@
         <v>1</v>
       </c>
       <c r="H213" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15697,7 +15715,7 @@
         <v>1</v>
       </c>
       <c r="H214" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15717,7 +15735,7 @@
         <v>8</v>
       </c>
       <c r="H215" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L215" s="0"/>
       <c r="M215" s="0"/>
@@ -15739,7 +15757,7 @@
         <v>1</v>
       </c>
       <c r="H216" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="L216" s="0"/>
       <c r="M216" s="0"/>
@@ -15749,7 +15767,7 @@
         <v>819</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>847</v>
@@ -15761,7 +15779,7 @@
         <v>2</v>
       </c>
       <c r="H217" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15769,7 +15787,7 @@
         <v>820</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C218" s="4" t="n">
         <v>0</v>
@@ -15840,7 +15858,7 @@
         <v>858</v>
       </c>
       <c r="H222" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15863,7 +15881,7 @@
         <v>858</v>
       </c>
       <c r="H223" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15886,7 +15904,7 @@
         <v>858</v>
       </c>
       <c r="H224" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15909,7 +15927,7 @@
         <v>858</v>
       </c>
       <c r="H225" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15931,7 +15949,7 @@
         <v>821</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C227" s="4" t="n">
         <v>0</v>
@@ -15945,7 +15963,7 @@
         <v>675</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C228" s="4" t="n">
         <v>0</v>
@@ -15959,7 +15977,7 @@
         <v>676</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C229" s="4" t="n">
         <v>0</v>
@@ -16088,7 +16106,7 @@
         <v>822</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>847</v>
@@ -16097,7 +16115,7 @@
         <v>1</v>
       </c>
       <c r="H238" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16154,7 +16172,7 @@
         <v>858</v>
       </c>
       <c r="H241" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16221,7 +16239,7 @@
         <v>823</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>851</v>
@@ -16233,7 +16251,7 @@
         <v>858</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16241,7 +16259,7 @@
         <v>824</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C247" s="4" t="n">
         <v>0</v>
@@ -16255,7 +16273,7 @@
         <v>825</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C248" s="4" t="n">
         <v>0</v>
@@ -16292,7 +16310,10 @@
         <v>1</v>
       </c>
       <c r="H250" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J250" s="4" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16312,7 +16333,7 @@
         <v>862</v>
       </c>
       <c r="H251" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16348,7 +16369,7 @@
         <v>826</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>847</v>
@@ -16357,7 +16378,7 @@
         <v>1</v>
       </c>
       <c r="H254" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16441,7 +16462,7 @@
         <v>827</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>847</v>
@@ -16450,7 +16471,7 @@
         <v>1</v>
       </c>
       <c r="H260" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16568,10 +16589,10 @@
         <v>2</v>
       </c>
       <c r="H268" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J268" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16588,7 +16609,10 @@
         <v>1</v>
       </c>
       <c r="H269" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J269" s="4" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16596,7 +16620,7 @@
         <v>828</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>847</v>
@@ -16605,7 +16629,10 @@
         <v>1</v>
       </c>
       <c r="H270" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J270" s="4" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16692,7 +16719,7 @@
         <v>829</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>847</v>
@@ -16734,7 +16761,7 @@
         <v>830</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C279" s="4" t="s">
         <v>847</v>
@@ -16743,7 +16770,7 @@
         <v>1</v>
       </c>
       <c r="H279" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16765,7 +16792,7 @@
         <v>831</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C281" s="4" t="s">
         <v>847</v>
@@ -16777,7 +16804,7 @@
         <v>1</v>
       </c>
       <c r="H281" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16800,7 +16827,7 @@
         <v>858</v>
       </c>
       <c r="H282" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16836,7 +16863,7 @@
         <v>832</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C285" s="4" t="s">
         <v>847</v>
@@ -16845,7 +16872,7 @@
         <v>1</v>
       </c>
       <c r="H285" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16881,7 +16908,7 @@
         <v>833</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C288" s="4" t="s">
         <v>847</v>
@@ -16890,7 +16917,7 @@
         <v>1</v>
       </c>
       <c r="H288" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16907,10 +16934,10 @@
         <v>2</v>
       </c>
       <c r="H289" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J289" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16927,7 +16954,10 @@
         <v>1</v>
       </c>
       <c r="H290" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
+      </c>
+      <c r="J290" s="4" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16944,7 +16974,7 @@
         <v>1</v>
       </c>
       <c r="H291" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16961,7 +16991,7 @@
         <v>1</v>
       </c>
       <c r="H292" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -16982,7 +17012,7 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -17094,7 +17124,7 @@
         <v>853</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17114,7 +17144,7 @@
         <v>853</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17131,7 +17161,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17148,7 +17178,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17165,7 +17195,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17182,7 +17212,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17199,10 +17229,10 @@
         <v>1</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17219,10 +17249,10 @@
         <v>1</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17239,10 +17269,10 @@
         <v>1</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17259,10 +17289,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17279,7 +17309,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17296,7 +17326,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17313,7 +17343,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17330,7 +17360,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17338,7 +17368,7 @@
         <v>879</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>851</v>
@@ -17347,10 +17377,10 @@
         <v>1</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17358,7 +17388,7 @@
         <v>880</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>851</v>
@@ -17367,10 +17397,10 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17378,7 +17408,7 @@
         <v>881</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>851</v>
@@ -17387,10 +17417,10 @@
         <v>1</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17398,7 +17428,7 @@
         <v>882</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>851</v>
@@ -17407,10 +17437,10 @@
         <v>1</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17418,19 +17448,19 @@
         <v>883</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>848</v>
-      </c>
-      <c r="C23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>849</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17438,19 +17468,19 @@
         <v>884</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>848</v>
-      </c>
-      <c r="C24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>849</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17458,19 +17488,19 @@
         <v>885</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>848</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>849</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17478,19 +17508,19 @@
         <v>886</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>848</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>849</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17507,7 +17537,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17524,7 +17554,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17541,7 +17571,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17558,7 +17588,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17566,7 +17596,7 @@
         <v>891</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>847</v>
@@ -17578,10 +17608,10 @@
         <v>1</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17589,7 +17619,7 @@
         <v>893</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>847</v>
@@ -17601,10 +17631,10 @@
         <v>1</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17612,7 +17642,7 @@
         <v>895</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>847</v>
@@ -17621,10 +17651,10 @@
         <v>1</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17632,7 +17662,7 @@
         <v>896</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>847</v>
@@ -17641,10 +17671,10 @@
         <v>1</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17661,7 +17691,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17678,7 +17708,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17698,7 +17728,7 @@
         <v>852</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17718,7 +17748,7 @@
         <v>852</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17735,7 +17765,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17752,7 +17782,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17760,7 +17790,7 @@
         <v>901</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>847</v>
@@ -17772,10 +17802,10 @@
         <v>1</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17783,7 +17813,7 @@
         <v>902</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>847</v>
@@ -17795,10 +17825,10 @@
         <v>1</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17815,7 +17845,7 @@
         <v>1</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17832,7 +17862,7 @@
         <v>1</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17849,7 +17879,7 @@
         <v>8</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17866,7 +17896,7 @@
         <v>5</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17883,7 +17913,7 @@
         <v>5</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17900,7 +17930,7 @@
         <v>8</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17920,7 +17950,7 @@
         <v>852</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17940,7 +17970,7 @@
         <v>852</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17960,7 +17990,7 @@
         <v>852</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17980,7 +18010,7 @@
         <v>913</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18000,7 +18030,7 @@
         <v>852</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18020,7 +18050,7 @@
         <v>852</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18037,7 +18067,7 @@
         <v>8</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18054,7 +18084,7 @@
         <v>8</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18071,7 +18101,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18088,7 +18118,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18105,7 +18135,7 @@
         <v>25</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18122,7 +18152,7 @@
         <v>25</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18139,7 +18169,7 @@
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18156,7 +18186,7 @@
         <v>2</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18176,7 +18206,7 @@
         <v>925</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18196,7 +18226,7 @@
         <v>925</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18213,7 +18243,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18230,7 +18260,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18238,7 +18268,7 @@
         <v>929</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>0</v>
@@ -18247,10 +18277,10 @@
         <v>4</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18258,7 +18288,7 @@
         <v>930</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>0</v>
@@ -18267,10 +18297,10 @@
         <v>4</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18278,7 +18308,7 @@
         <v>931</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>0</v>
@@ -18287,10 +18317,10 @@
         <v>15</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18298,7 +18328,7 @@
         <v>932</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>0</v>
@@ -18307,10 +18337,10 @@
         <v>15</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18333,7 +18363,7 @@
         <v>855</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18350,7 +18380,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18373,7 +18403,7 @@
         <v>855</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18381,7 +18411,7 @@
         <v>744</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>854</v>
@@ -18396,10 +18426,10 @@
         <v>855</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18422,7 +18452,7 @@
         <v>855</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18430,7 +18460,7 @@
         <v>745</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>854</v>
@@ -18445,10 +18475,10 @@
         <v>855</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18471,7 +18501,7 @@
         <v>855</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
   </sheetData>
@@ -33223,8 +33253,8 @@
   </sheetPr>
   <dimension ref="A1:G709"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A125" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D140" activeCellId="0" sqref="D140"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A328" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I335" activeCellId="0" sqref="I335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
split prbs read procedure for v7 and usplus families, fixed small bug originating from Xilinx GTY datasheet
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
+++ b/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="US+_GTY_tx_rx" sheetId="1" state="visible" r:id="rId2"/>
@@ -11618,7 +11618,7 @@
   </sheetPr>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -33253,8 +33253,8 @@
   </sheetPr>
   <dimension ref="A1:G709"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A328" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I335" activeCellId="0" sqref="I335"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A519" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H546" activeCellId="0" sqref="H546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39460,7 +39460,7 @@
         <v>1209</v>
       </c>
       <c r="B546" s="3" t="s">
-        <v>968</v>
+        <v>1001</v>
       </c>
       <c r="C546" s="3" t="s">
         <v>942</v>

</xml_diff>

<commit_message>
moved manually created refclk_buf SV source into XLSX sources
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
+++ b/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="US+_GTY_tx_rx" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="xcku15p-ffva1760_GTY_placement" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="US+_GTY_quad_connections" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="US+_GTY_mgt_config" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="refclk_buf" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="1607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7063" uniqueCount="1621">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -4848,6 +4849,48 @@
   </si>
   <si>
     <t xml:space="preserve">name of QPLL power down port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refclk_buf_inst.sv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBUFDS_GTE4 #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.REFCLK_EN_TX_PATH  (1'b0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.REFCLK_HROW_CK_SEL (2'b00),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.REFCLK_ICNTL_RX    (2'b00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">refclk_buf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.I     (refclk_p [gi]),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.IB    (refclk_n [gi]),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.CEB   (1'b0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.O     (refclk   [gi]),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.ODIV2 ()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">);</t>
   </si>
 </sst>
 </file>
@@ -4858,7 +4901,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4891,6 +4934,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -4936,7 +4985,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4981,6 +5030,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -5000,7 +5053,7 @@
   </sheetPr>
   <dimension ref="A1:F829"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -11618,7 +11671,7 @@
   </sheetPr>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -17012,7 +17065,7 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -18522,7 +18575,7 @@
   </sheetPr>
   <dimension ref="A1:G901"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D278" activeCellId="0" sqref="D278"/>
     </sheetView>
   </sheetViews>
@@ -33253,7 +33306,7 @@
   </sheetPr>
   <dimension ref="A1:G709"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A519" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A519" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H546" activeCellId="0" sqref="H546"/>
     </sheetView>
   </sheetViews>
@@ -41333,7 +41386,7 @@
   </sheetPr>
   <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -44654,7 +44707,7 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -45013,8 +45066,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -45313,4 +45366,129 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="31.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="11" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="11" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="11" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="11" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="11" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="11" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="11" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="11" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="11" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="11" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="11" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="11" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="11" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="11" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added back missing polarity port names, removed by mistake
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
+++ b/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="US+_GTY_tx_rx" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7216" uniqueCount="1636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7222" uniqueCount="1640">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -4863,6 +4863,18 @@
   </si>
   <si>
     <t xml:space="preserve">name of RX user clock port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mgt_txpolarity_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name of TX polarity port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mgt_rxpolarity_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name of RX polarity port</t>
   </si>
   <si>
     <t xml:space="preserve">refclk_buf_inst.sv</t>
@@ -5105,7 +5117,7 @@
   <dimension ref="A1:F829"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E125:E128 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11723,7 +11735,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="1" sqref="E125:E128 E20"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11748,7 +11760,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1611</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11761,72 +11773,72 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="11" t="s">
-        <v>1612</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="11" t="s">
-        <v>1613</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="11" t="s">
-        <v>1614</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="11" t="s">
-        <v>1615</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="11" t="s">
-        <v>1616</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="11" t="s">
-        <v>1617</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="11" t="s">
-        <v>1618</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="11" t="s">
-        <v>1613</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="11" t="s">
-        <v>1619</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="11" t="s">
-        <v>1620</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="11" t="s">
-        <v>1621</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="11" t="s">
-        <v>1622</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="11" t="s">
-        <v>1623</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="11" t="s">
-        <v>1624</v>
+        <v>1628</v>
       </c>
     </row>
   </sheetData>
@@ -11848,7 +11860,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="E125:E128 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11858,12 +11870,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1625</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1626</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11893,7 +11905,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1627</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11901,7 +11913,7 @@
         <v>856</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>1628</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11909,7 +11921,7 @@
         <v>851</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1629</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11917,7 +11929,7 @@
         <v>854</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>1630</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11925,7 +11937,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1631</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11933,22 +11945,22 @@
         <v>847</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1632</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1633</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1634</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1635</v>
+        <v>1639</v>
       </c>
     </row>
   </sheetData>
@@ -11970,7 +11982,7 @@
   <dimension ref="A1:M292"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="1" sqref="E125:E128 H38"/>
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17370,7 +17382,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="1" sqref="E125:E128 F39"/>
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18886,7 +18898,7 @@
   <dimension ref="A1:G901"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D278" activeCellId="1" sqref="E125:E128 D278"/>
+      <selection pane="topLeft" activeCell="D278" activeCellId="0" sqref="D278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33617,7 +33629,7 @@
   <dimension ref="A1:G709"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A519" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H546" activeCellId="1" sqref="E125:E128 H546"/>
+      <selection pane="topLeft" activeCell="H546" activeCellId="0" sqref="H546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41697,7 +41709,7 @@
   <dimension ref="A1:Q132"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E125:E128 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -46396,8 +46408,8 @@
   </sheetPr>
   <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E125" activeCellId="0" sqref="E125:E128"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E125" activeCellId="0" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -50971,7 +50983,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E125:E128 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -51327,10 +51339,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="E125:E128 B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -51554,8 +51566,28 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>646</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>1614</v>
+      </c>
+    </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
CPLLRESET was hardcoded, made accessible now
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
+++ b/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="US+_GTY_tx_rx" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7238" uniqueCount="1649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7240" uniqueCount="1649">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -12127,8 +12127,8 @@
   </sheetPr>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12463,11 +12463,14 @@
       <c r="B16" s="4" t="s">
         <v>845</v>
       </c>
-      <c r="C16" s="4" t="n">
-        <v>0</v>
+      <c r="C16" s="4" t="s">
+        <v>847</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>850</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="5"/>
@@ -41854,7 +41857,7 @@
   </sheetPr>
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed mgt_rxsyncallin signal that was not indexed
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
+++ b/examples/vu13p_25g_all/src/xcvu13p-fsga2577.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7242" uniqueCount="1651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7243" uniqueCount="1651">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -12129,8 +12129,8 @@
   </sheetPr>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A178" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H206" activeCellId="0" sqref="H206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16092,6 +16092,9 @@
       </c>
       <c r="E205" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="H205" s="4" t="s">
+        <v>851</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19054,8 +19057,8 @@
   </sheetPr>
   <dimension ref="A1:G901"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D278" activeCellId="0" sqref="D278"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A694" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F722" activeCellId="0" sqref="F722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>